<commit_message>
adding location and fix navbar
</commit_message>
<xml_diff>
--- a/public/todo.xlsx
+++ b/public/todo.xlsx
@@ -674,7 +674,7 @@
   <dimension ref="C2:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -880,8 +880,8 @@
       <c r="C17" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="6" t="s">
-        <v>14</v>
+      <c r="D17" s="5" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.3">

</xml_diff>